<commit_message>
doc(journal de travail): Ajout des heures de travails du 18.11.2024
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Botteau_Mathis_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Botteau_Mathis_Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd47qky\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC75104F-6D8B-48E5-A4D0-0A1FAAC47478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98690C4-9D29-4413-851E-770406CCA7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Auteur:</t>
   </si>
@@ -134,6 +134,18 @@
   </si>
   <si>
     <t>18.11.2024  au 10.01.2025</t>
+  </si>
+  <si>
+    <t>Plannification du projet</t>
+  </si>
+  <si>
+    <t>Je me suis informé sur les test unitaires backend JS, et sur les outils Jest et supertest</t>
+  </si>
+  <si>
+    <t>Analyse de la politique de test, quel outils, envirronements, tests</t>
+  </si>
+  <si>
+    <t>Création d'un docker compose avec docker file afin de faire tourner l'application sur docker</t>
   </si>
 </sst>
 </file>
@@ -1083,10 +1095,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1935,10 +1947,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.69444444444444442</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.30555555555555558</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4130,7 +4142,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4185,7 +4197,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>0 heures 0 minutes</v>
+        <v>3 heures 0 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4204,11 +4216,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4243,27 +4255,43 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="str">
+      <c r="A7" s="72">
         <f>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</f>
-        <v/>
-      </c>
-      <c r="B7" s="32"/>
+        <v>47</v>
+      </c>
+      <c r="B7" s="32">
+        <v>45614</v>
+      </c>
       <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="28"/>
+      <c r="D7" s="34">
+        <v>35</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>31</v>
+      </c>
       <c r="G7" s="44"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="73" t="str">
+      <c r="A8" s="73">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v/>
-      </c>
-      <c r="B8" s="36"/>
+        <v>47</v>
+      </c>
+      <c r="B8" s="36">
+        <v>45614</v>
+      </c>
       <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="28"/>
+      <c r="D8" s="38">
+        <v>45</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>32</v>
+      </c>
       <c r="G8" s="45"/>
       <c r="M8" t="s">
         <v>2</v>
@@ -4276,15 +4304,23 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="74" t="str">
+      <c r="A9" s="74">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="40"/>
+        <v>47</v>
+      </c>
+      <c r="B9" s="40">
+        <v>45614</v>
+      </c>
       <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="28"/>
+      <c r="D9" s="42">
+        <v>45</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>33</v>
+      </c>
       <c r="G9" s="46"/>
       <c r="M9" t="s">
         <v>19</v>
@@ -4297,15 +4333,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="str">
+      <c r="A10" s="73">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="36"/>
+        <v>47</v>
+      </c>
+      <c r="B10" s="36">
+        <v>45614</v>
+      </c>
       <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="28"/>
+      <c r="D10" s="38">
+        <v>55</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>34</v>
+      </c>
       <c r="G10" s="45"/>
       <c r="M10" t="s">
         <v>3</v>
@@ -10766,11 +10810,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10778,11 +10822,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
-      </c>
-      <c r="G6" s="47" t="e">
+        <v>2 h 05 min</v>
+      </c>
+      <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>#DIV/0!</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10803,11 +10847,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10815,11 +10859,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
-      </c>
-      <c r="G7" s="56" t="e">
+        <v>0 h 55 min</v>
+      </c>
+      <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>#DIV/0!</v>
+        <v>0.30555555555555558</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10854,9 +10898,9 @@
         <f t="shared" si="1"/>
         <v>0 h 00 min</v>
       </c>
-      <c r="G8" s="47" t="e">
+      <c r="G8" s="47">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L8" s="65" t="str">
         <f>'Journal de travail'!M10</f>
@@ -10891,9 +10935,9 @@
         <f t="shared" si="1"/>
         <v>0 h 00 min</v>
       </c>
-      <c r="G9" s="56" t="e">
+      <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10914,22 +10958,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 00 min</v>
+        <v>3 h 00 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0</v>
+        <v>3.4090909090909088E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -10973,26 +11017,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11215,32 +11239,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11257,4 +11276,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(Journal de travail): Ajout des heures de travails du 02.12.2024
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Botteau_Mathis_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Botteau_Mathis_Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd47qky\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98690C4-9D29-4413-851E-770406CCA7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B647738-28F2-4619-AC95-C317D5C2183B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Auteur:</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>Création d'un docker compose avec docker file afin de faire tourner l'application sur docker</t>
+  </si>
+  <si>
+    <t>Analyse des tests avenir (plan de test)</t>
+  </si>
+  <si>
+    <t>Création des tests unitaires pour le backend de la route AUTH, connexion avec un user valide et invalide</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1101,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>125</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1947,10 +1953,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.69444444444444442</c:v>
+                  <c:v>0.65686274509803921</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.30555555555555558</c:v>
+                  <c:v>0.34313725490196079</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4142,7 +4148,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4197,7 +4203,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>3 heures 0 minutes</v>
+        <v>8 heures 30 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4212,15 +4218,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>180</v>
+        <v>510</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4362,15 +4368,25 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="str">
+      <c r="A11" s="74">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="28"/>
+        <v>48</v>
+      </c>
+      <c r="B11" s="40">
+        <v>45621</v>
+      </c>
+      <c r="C11" s="41">
+        <v>2</v>
+      </c>
+      <c r="D11" s="42">
+        <v>30</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="G11" s="46"/>
       <c r="M11" t="s">
         <v>4</v>
@@ -4383,15 +4399,25 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="str">
+      <c r="A12" s="73">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="28"/>
+        <v>49</v>
+      </c>
+      <c r="B12" s="36">
+        <v>45628</v>
+      </c>
+      <c r="C12" s="37">
+        <v>1</v>
+      </c>
+      <c r="D12" s="38">
+        <v>0</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="G12" s="45"/>
       <c r="N12">
         <v>5</v>
@@ -4400,16 +4426,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="str">
+    <row r="13" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="74">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="28"/>
+        <v>49</v>
+      </c>
+      <c r="B13" s="40">
+        <v>45628</v>
+      </c>
+      <c r="C13" s="41">
+        <v>2</v>
+      </c>
+      <c r="D13" s="42">
+        <v>0</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>36</v>
+      </c>
       <c r="G13" s="46"/>
       <c r="N13">
         <v>6</v>
@@ -10806,15 +10842,15 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>125</v>
+        <v>335</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10822,11 +10858,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>2 h 05 min</v>
+        <v>5 h 35 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.69444444444444442</v>
+        <v>0.65686274509803921</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10843,7 +10879,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
@@ -10851,7 +10887,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>175</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10859,11 +10895,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 55 min</v>
+        <v>2 h 55 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.30555555555555558</v>
+        <v>0.34313725490196079</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10954,26 +10990,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>180</v>
+        <v>510</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>3 h 00 min</v>
+        <v>8 h 30 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>3.4090909090909088E-2</v>
+        <v>9.6590909090909088E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11017,6 +11053,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11239,27 +11295,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11276,29 +11337,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(journal de travail): Ajout des heures de travail du 09.12.2024
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Botteau_Mathis_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Botteau_Mathis_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd47qky\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B647738-28F2-4619-AC95-C317D5C2183B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CD71FD-DEAC-4F02-A0F4-26DB36B6D75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Auteur:</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Création des tests unitaires pour le backend de la route AUTH, connexion avec un user valide et invalide</t>
+  </si>
+  <si>
+    <t>Création des tests End to End, login/logout et signup</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1107,7 @@
                   <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>175</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1953,10 +1956,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.65686274509803921</c:v>
+                  <c:v>0.55833333333333335</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.34313725490196079</c:v>
+                  <c:v>0.44166666666666665</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4148,7 +4151,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4203,7 +4206,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>8 heures 30 minutes</v>
+        <v>10 heures 0 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4218,15 +4221,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>510</v>
+        <v>600</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4455,15 +4458,25 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="str">
+      <c r="A14" s="73">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="28"/>
+        <v>50</v>
+      </c>
+      <c r="B14" s="36">
+        <v>45635</v>
+      </c>
+      <c r="C14" s="37">
+        <v>1</v>
+      </c>
+      <c r="D14" s="38">
+        <v>30</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>37</v>
+      </c>
       <c r="G14" s="45"/>
       <c r="N14">
         <v>7</v>
@@ -10862,7 +10875,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.65686274509803921</v>
+        <v>0.55833333333333335</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10879,15 +10892,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>265</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10895,11 +10908,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>2 h 55 min</v>
+        <v>4 h 25 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.34313725490196079</v>
+        <v>0.44166666666666665</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10990,26 +11003,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>510</v>
+        <v>600</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>8 h 30 min</v>
+        <v>10 h 00 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>9.6590909090909088E-2</v>
+        <v>0.11363636363636363</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11053,26 +11066,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11295,32 +11288,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11337,4 +11325,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(journal de travail): Ajout des heures de travail du 13.12.2024
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Botteau_Mathis_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Botteau_Mathis_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd47qky\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CD71FD-DEAC-4F02-A0F4-26DB36B6D75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3C0A59-67FE-4773-BA4F-0D578437AA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Auteur:</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Création des tests End to End, login/logout et signup</t>
+  </si>
+  <si>
+    <t>Création des test cypress, login/logout, gestions todso, gestion profile, ajout todo</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1110,7 @@
                   <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>265</c:v>
+                  <c:v>445</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1956,10 +1959,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.55833333333333335</c:v>
+                  <c:v>0.42948717948717946</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44166666666666665</c:v>
+                  <c:v>0.57051282051282048</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4151,7 +4154,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4206,7 +4209,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>10 heures 0 minutes</v>
+        <v>13 heures 0 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4221,7 +4224,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>540</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -4229,7 +4232,7 @@
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>600</v>
+        <v>780</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4486,15 +4489,25 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="str">
+      <c r="A15" s="74">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="28"/>
+        <v>50</v>
+      </c>
+      <c r="B15" s="40">
+        <v>45639</v>
+      </c>
+      <c r="C15" s="41">
+        <v>3</v>
+      </c>
+      <c r="D15" s="42">
+        <v>0</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="G15" s="46"/>
       <c r="N15">
         <v>8</v>
@@ -10875,7 +10888,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.55833333333333335</v>
+        <v>0.42948717948717946</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10892,7 +10905,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
@@ -10900,7 +10913,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>265</v>
+        <v>445</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10908,11 +10921,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>4 h 25 min</v>
+        <v>7 h 25 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.44166666666666665</v>
+        <v>0.57051282051282048</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11003,7 +11016,7 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>360</v>
+        <v>540</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
@@ -11011,18 +11024,18 @@
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>600</v>
+        <v>780</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>10 h 00 min</v>
+        <v>13 h 00 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.11363636363636363</v>
+        <v>0.14772727272727273</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11066,6 +11079,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11288,27 +11321,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11325,29 +11363,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(journal de travail): Ajout des heures de travail du  16.12.2024
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Botteau_Mathis_Test.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Botteau_Mathis_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd47qky\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3C0A59-67FE-4773-BA4F-0D578437AA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A3A2B2-6750-44DF-A35F-2C9C656F6665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Auteur:</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Création des test cypress, login/logout, gestions todso, gestion profile, ajout todo</t>
+  </si>
+  <si>
+    <t>Auto évaluation</t>
+  </si>
+  <si>
+    <t>Création des test cypress, gestion de profil, supression de compte, navigation</t>
   </si>
 </sst>
 </file>
@@ -289,7 +295,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF569CD6"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -584,10 +589,6 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -597,6 +598,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1107,10 +1112,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>335</c:v>
+                  <c:v>365</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>445</c:v>
+                  <c:v>595</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1959,10 +1964,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.42948717948717946</c:v>
+                  <c:v>0.38020833333333331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57051282051282048</c:v>
+                  <c:v>0.61979166666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4154,7 +4159,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4186,15 +4191,15 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="81" t="s">
+      <c r="B2" s="82"/>
+      <c r="C2" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
@@ -4203,13 +4208,13 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="83"/>
+      <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>13 heures 0 minutes</v>
+        <v>16 heures 0 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4224,24 +4229,24 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>540</v>
+        <v>660</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>780</v>
+        <v>960</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="82"/>
+      <c r="D5" s="81"/>
     </row>
     <row r="6" spans="1:15" s="17" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
@@ -4517,30 +4522,48 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="73" t="str">
+      <c r="A16" s="73">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="28"/>
+        <v>51</v>
+      </c>
+      <c r="B16" s="36">
+        <v>45642</v>
+      </c>
+      <c r="C16" s="37">
+        <v>2</v>
+      </c>
+      <c r="D16" s="38">
+        <v>30</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>40</v>
+      </c>
       <c r="G16" s="45"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="74" t="str">
+      <c r="A17" s="74">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="40"/>
+        <v>51</v>
+      </c>
+      <c r="B17" s="40">
+        <v>45642</v>
+      </c>
       <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="80"/>
+      <c r="D17" s="42">
+        <v>30</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="83" t="s">
+        <v>39</v>
+      </c>
       <c r="G17" s="46"/>
       <c r="O17">
         <v>45</v>
@@ -10872,11 +10895,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>335</v>
+        <v>365</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10884,11 +10907,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>5 h 35 min</v>
+        <v>6 h 05 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.42948717948717946</v>
+        <v>0.38020833333333331</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10905,15 +10928,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>445</v>
+        <v>595</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10921,11 +10944,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>7 h 25 min</v>
+        <v>9 h 55 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.57051282051282048</v>
+        <v>0.61979166666666663</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11016,26 +11039,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>540</v>
+        <v>660</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>780</v>
+        <v>960</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>13 h 00 min</v>
+        <v>16 h 00 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.14772727272727273</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11079,26 +11102,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11321,32 +11324,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11363,4 +11361,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>